<commit_message>
added 2 number additions in excel.
</commit_message>
<xml_diff>
--- a/TimberBeamCalculator/TimberBeamData.xlsx
+++ b/TimberBeamCalculator/TimberBeamData.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="myRange1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -367,15 +367,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -383,7 +383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -393,13 +393,25 @@
       <c r="C2">
         <v>4.55</v>
       </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f>SUM(E2:E3)</f>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pass in a cell value from excel to pdf due to cell being red.
</commit_message>
<xml_diff>
--- a/TimberBeamCalculator/TimberBeamData.xlsx
+++ b/TimberBeamCalculator/TimberBeamData.xlsx
@@ -23,10 +23,23 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -52,8 +65,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,35 +373,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4.5599999999999996</v>
       </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7.89</v>
+      </c>
+      <c r="B4" s="1">
+        <f>SUM(B2:B3)</f>
+        <v>5</v>
+      </c>
+      <c r="C4" s="2">
+        <f>AVERAGE(C2:C3)</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
extract calculated excel value out part 2
</commit_message>
<xml_diff>
--- a/TimberBeamCalculator/TimberBeamData.xlsx
+++ b/TimberBeamCalculator/TimberBeamData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
-  </bookViews>
-  <sheets>
-    <sheet name="myRange1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="152511"/>
-</workbook>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
+  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <x:workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <x:bookViews>
+    <x:workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="myRange1" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:calcPr calcId="152511" fullCalcOnLoad="1" forceFullCalc="1"/>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -372,57 +372,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4.5599999999999996</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>7.89</v>
-      </c>
-      <c r="B4" s="1">
-        <f>SUM(B2:B3)</f>
-        <v>5</v>
-      </c>
-      <c r="C4" s="2">
-        <f>AVERAGE(C2:C3)</f>
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:dimension ref="A1:C6"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="I16" sqref="I16"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A2">
+        <x:v>5.6</x:v>
+      </x:c>
+      <x:c r="B2">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="C2">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A3">
+        <x:v>4.5599999999999996</x:v>
+      </x:c>
+      <x:c r="B3">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C3">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A4">
+        <x:v>7.89</x:v>
+      </x:c>
+      <x:c r="B4" s="1">
+        <x:f>SUM(B2:B3)</x:f>
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C4" s="2">
+        <x:f>SUM(C2:C3)</x:f>
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="C6">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
recalculating excel formula cell after values are entered.
</commit_message>
<xml_diff>
--- a/TimberBeamCalculator/TimberBeamData.xlsx
+++ b/TimberBeamCalculator/TimberBeamData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
-  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <x:workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <x:bookViews>
-    <x:workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="myRange1" sheetId="1" r:id="rId1"/>
-  </x:sheets>
-  <x:calcPr calcId="152511" fullCalcOnLoad="1" forceFullCalc="1"/>
-</x:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+  </bookViews>
+  <sheets>
+    <sheet name="myRange1" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="152511" forceFullCalc="1"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -372,62 +372,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <x:dimension ref="A1:C6"/>
-  <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="I16" sqref="I16"/>
-    </x:sheetView>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A1" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A2">
-        <x:v>5.6</x:v>
-      </x:c>
-      <x:c r="B2">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="C2">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A3">
-        <x:v>4.5599999999999996</x:v>
-      </x:c>
-      <x:c r="B3">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C3">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A4">
-        <x:v>7.89</x:v>
-      </x:c>
-      <x:c r="B4" s="1">
-        <x:f>SUM(B2:B3)</x:f>
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="C4" s="2">
-        <x:f>SUM(C2:C3)</x:f>
-        <x:v>17</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="C6">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <x:pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5.6</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>7.89</v>
+      </c>
+      <c r="B4" s="1">
+        <f>SUM(B2:B3)</f>
+        <v>5</v>
+      </c>
+      <c r="C4" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <f>SUM(C2:C4)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add 2 numbers from screen and send the sum in pdf part 1
</commit_message>
<xml_diff>
--- a/TimberBeamCalculator/TimberBeamData.xlsx
+++ b/TimberBeamCalculator/TimberBeamData.xlsx
@@ -1,89 +1,121 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
-  </bookViews>
-  <sheets>
-    <sheet name="myRange1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="152511" forceFullCalc="1"/>
-</workbook>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
+  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <x:workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <x:bookViews>
+    <x:workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="0" activeTab="0"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="myRange1" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="152511" forceFullCalc="1"/>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>FirstName</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <x:si>
+    <x:t>FirstName</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="5" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:sz val="11"/>
+      <x:color rgb="FFFF0000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="3">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="5">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -372,67 +404,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5.6</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4.5599999999999996</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>7.89</v>
-      </c>
-      <c r="B4" s="1">
-        <f>SUM(B2:B3)</f>
-        <v>5</v>
-      </c>
-      <c r="C4" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <f>SUM(C2:C4)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:G6"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="C4" sqref="C4 C4:C4"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="3" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="3" t="n">
+        <x:v>5.6</x:v>
+      </x:c>
+      <x:c r="B2" s="3" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="C2" s="3" t="n">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="3" t="n">
+        <x:v>4.56</x:v>
+      </x:c>
+      <x:c r="B3" s="3" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C3" s="3" t="n">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="3" t="n">
+        <x:v>7.89</x:v>
+      </x:c>
+      <x:c r="B4" s="4">
+        <x:f>SUM(B2:B3)</x:f>
+      </x:c>
+      <x:c r="C4" s="3">
+        <x:f>SUM(C2:C3)</x:f>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <x:c r="C6" s="3" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="G6" s="3" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" horizontalDpi="300" verticalDpi="300"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>